<commit_message>
Added custom duration and task interactive tasks
</commit_message>
<xml_diff>
--- a/GestorPAT/src/td/fileProcess.xlsx
+++ b/GestorPAT/src/td/fileProcess.xlsx
@@ -3,24 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{713CEC63-61B4-4AE2-867D-5369DFF8F80A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C3FCDB24-C239-408B-B433-D655EEFFDBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="14400" windowHeight="7800" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="14400" windowHeight="7800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Process 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Process 2" sheetId="2" r:id="rId2"/>
-    <sheet name="Process 3" sheetId="3" r:id="rId3"/>
-    <sheet name="Process 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Process 5" sheetId="5" r:id="rId5"/>
+    <sheet name="P-1" sheetId="1" r:id="rId1"/>
+    <sheet name="P-2" sheetId="2" r:id="rId2"/>
+    <sheet name="P-3" sheetId="3" r:id="rId3"/>
+    <sheet name="P-4" sheetId="4" r:id="rId4"/>
+    <sheet name="P-5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M11"/>
+  <oleSize ref="A1:M18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -40,148 +40,226 @@
     <t>01</t>
   </si>
   <si>
-    <t>Process 1</t>
+    <t>P-1</t>
   </si>
   <si>
     <t>Testing process 1</t>
   </si>
   <si>
+    <t>Running</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Activity ID</t>
+  </si>
+  <si>
+    <t>Activity Name</t>
+  </si>
+  <si>
+    <t>Activity Description</t>
+  </si>
+  <si>
+    <t>Activity State</t>
+  </si>
+  <si>
+    <t>Activity Owner</t>
+  </si>
+  <si>
+    <t>427</t>
+  </si>
+  <si>
+    <t>A3-1</t>
+  </si>
+  <si>
+    <t>Testing 3</t>
+  </si>
+  <si>
+    <t>Task ID</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Task Description</t>
+  </si>
+  <si>
+    <t>Task State</t>
+  </si>
+  <si>
+    <t>Task Owner</t>
+  </si>
+  <si>
+    <t>Task Duration</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>Task 1</t>
+  </si>
+  <si>
+    <t>Testing 1</t>
+  </si>
+  <si>
+    <t>PT3M44S</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>741</t>
+  </si>
+  <si>
+    <t>Task 2</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>PT0S</t>
+  </si>
+  <si>
+    <t>344</t>
+  </si>
+  <si>
+    <t>Task 3</t>
+  </si>
+  <si>
+    <t>PT58M56S</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>A4-1</t>
+  </si>
+  <si>
+    <t>Testing 4</t>
+  </si>
+  <si>
+    <t>1534</t>
+  </si>
+  <si>
+    <t>T1-4-1</t>
+  </si>
+  <si>
     <t>Ready</t>
   </si>
   <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Activity ID</t>
-  </si>
-  <si>
-    <t>Activity Name</t>
-  </si>
-  <si>
-    <t>Activity Description</t>
-  </si>
-  <si>
-    <t>Activity State</t>
-  </si>
-  <si>
-    <t>Activity Owner</t>
-  </si>
-  <si>
-    <t>Activity 1</t>
+    <t>PT1H49M13S</t>
+  </si>
+  <si>
+    <t>1589</t>
+  </si>
+  <si>
+    <t>A2-1</t>
+  </si>
+  <si>
+    <t>Testing activity 2</t>
+  </si>
+  <si>
+    <t>631</t>
+  </si>
+  <si>
+    <t>T2-2-1</t>
+  </si>
+  <si>
+    <t>Testing 2</t>
+  </si>
+  <si>
+    <t>PT19M38S</t>
+  </si>
+  <si>
+    <t>705</t>
+  </si>
+  <si>
+    <t>T1-1-1</t>
+  </si>
+  <si>
+    <t>A1-1</t>
   </si>
   <si>
     <t>Testing activity 1</t>
   </si>
   <si>
-    <t>Task ID</t>
-  </si>
-  <si>
-    <t>Task Name</t>
-  </si>
-  <si>
-    <t>Task Description</t>
-  </si>
-  <si>
-    <t>Task State</t>
-  </si>
-  <si>
-    <t>Task Owner</t>
-  </si>
-  <si>
-    <t>Task Duration</t>
-  </si>
-  <si>
-    <t>Mandatory</t>
-  </si>
-  <si>
     <t>1995</t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Testing 1</t>
-  </si>
-  <si>
-    <t>Running</t>
-  </si>
-  <si>
-    <t>PT15M</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>329</t>
   </si>
   <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Testing 2</t>
+    <t>02</t>
+  </si>
+  <si>
+    <t>P-2</t>
+  </si>
+  <si>
+    <t>Testing process 2</t>
+  </si>
+  <si>
+    <t>454</t>
+  </si>
+  <si>
+    <t>Act 1-2</t>
+  </si>
+  <si>
+    <t>Testing 1-2</t>
+  </si>
+  <si>
+    <t>763</t>
+  </si>
+  <si>
+    <t>Task 1-1-2</t>
+  </si>
+  <si>
+    <t>Testing 1-1-2</t>
+  </si>
+  <si>
+    <t>PT1H33M45S</t>
+  </si>
+  <si>
+    <t>1044</t>
+  </si>
+  <si>
+    <t>Act 2-2</t>
+  </si>
+  <si>
+    <t>Testing 2-2</t>
   </si>
   <si>
     <t>Blocked</t>
   </si>
   <si>
-    <t>1589</t>
-  </si>
-  <si>
-    <t>Activity 2</t>
-  </si>
-  <si>
-    <t>Testing activity 2</t>
-  </si>
-  <si>
-    <t>631</t>
-  </si>
-  <si>
-    <t>PT30M</t>
-  </si>
-  <si>
-    <t>705</t>
-  </si>
-  <si>
-    <t>427</t>
-  </si>
-  <si>
-    <t>Activity 3</t>
-  </si>
-  <si>
-    <t>Testing 3</t>
-  </si>
-  <si>
-    <t>231</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>Activity 4</t>
-  </si>
-  <si>
-    <t>Testing 4</t>
-  </si>
-  <si>
-    <t>1534</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>Process 2</t>
-  </si>
-  <si>
-    <t>Testing process 2</t>
+    <t>1415</t>
+  </si>
+  <si>
+    <t>Task 2-1-2</t>
+  </si>
+  <si>
+    <t>Testing 2-1-2</t>
+  </si>
+  <si>
+    <t>PT3M45S</t>
+  </si>
+  <si>
+    <t>1939</t>
+  </si>
+  <si>
+    <t>Act 3-2</t>
+  </si>
+  <si>
+    <t>Testing 3-2</t>
   </si>
   <si>
     <t>03</t>
   </si>
   <si>
-    <t>Process 3</t>
+    <t>P-3</t>
   </si>
   <si>
     <t>Testing process 3</t>
@@ -190,22 +268,22 @@
     <t>04</t>
   </si>
   <si>
-    <t>Process 4</t>
+    <t>P-4</t>
   </si>
   <si>
     <t>Testing process 4</t>
   </si>
   <si>
-    <t>Exit</t>
-  </si>
-  <si>
     <t>1694</t>
   </si>
   <si>
-    <t>Process 5</t>
+    <t>P-5</t>
   </si>
   <si>
     <t>Testing 5</t>
+  </si>
+  <si>
+    <t>Finished</t>
   </si>
 </sst>
 </file>
@@ -557,9 +635,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -616,13 +696,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -633,39 +713,39 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -688,13 +768,13 @@
         <v>32</v>
       </c>
       <c r="D7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
         <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -708,36 +788,42 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
+      <c r="G8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -745,45 +831,39 @@
         <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -794,122 +874,191 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
         <v>42</v>
       </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
       <c r="E12" t="s">
         <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="G14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
         <v>26</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C19" t="s">
         <v>27</v>
       </c>
-      <c r="E17" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
+      <c r="D19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -919,13 +1068,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,24 +1091,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -974,6 +1123,172 @@
       </c>
       <c r="E3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1008,16 +1323,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -1072,16 +1387,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -1136,16 +1451,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>

</xml_diff>